<commit_message>
Added Smartphone Addicted Population
</commit_message>
<xml_diff>
--- a/Copy of IS Observation Form 2024 (Responses).xlsx
+++ b/Copy of IS Observation Form 2024 (Responses).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nabtang\Documents\GitHub\IS-Observation-Form-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BE3379-6509-4344-A690-9BECC86274C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF647532-D9A7-48A9-81D0-D21FE98FE21C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4344" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4346" uniqueCount="456">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1488,6 +1488,12 @@
   <si>
     <t>Sigma Red</t>
   </si>
+  <si>
+    <t>Phone Addicted Male ()</t>
+  </si>
+  <si>
+    <t>Phone Addicted Female ()</t>
+  </si>
 </sst>
 </file>
 
@@ -1834,11 +1840,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AW441"/>
+  <dimension ref="A1:AZ441"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AU1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AU342" sqref="AU342"/>
+      <selection pane="bottomLeft" activeCell="AY14" sqref="AY14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1864,10 +1870,13 @@
     <col min="40" max="44" width="18.85546875" customWidth="1"/>
     <col min="45" max="45" width="26" customWidth="1"/>
     <col min="46" max="46" width="120.140625" customWidth="1"/>
-    <col min="47" max="53" width="18.85546875" customWidth="1"/>
+    <col min="47" max="50" width="18.85546875" customWidth="1"/>
+    <col min="51" max="51" width="28" customWidth="1"/>
+    <col min="52" max="52" width="26.42578125" customWidth="1"/>
+    <col min="53" max="53" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2013,7 +2022,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A2" s="10">
         <v>45509.701037893523</v>
       </c>
@@ -2157,8 +2166,14 @@
         <f>SUM(G2:Q2)</f>
         <v>16</v>
       </c>
+      <c r="AY2" t="s">
+        <v>454</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>455</v>
+      </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
         <v>45509.70180761574</v>
       </c>
@@ -2302,8 +2317,16 @@
         <f>SUM(G3:Q3)</f>
         <v>21</v>
       </c>
+      <c r="AY3">
+        <f>COUNTIF(AW2:AW142,"&gt;=31")</f>
+        <v>63</v>
+      </c>
+      <c r="AZ3">
+        <f>COUNTIF(AW143:AW341,"&gt;=33")</f>
+        <v>86</v>
+      </c>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
         <v>45510.305194814813</v>
       </c>
@@ -2448,7 +2471,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
         <v>45510.305908900467</v>
       </c>
@@ -2593,7 +2616,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A6" s="10">
         <v>45510.450860081022</v>
       </c>
@@ -2738,7 +2761,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A7" s="10">
         <v>45533.454514236109</v>
       </c>
@@ -2883,7 +2906,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
         <v>45534.598930266206</v>
       </c>
@@ -3028,7 +3051,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
         <v>45510.304203993059</v>
       </c>
@@ -3173,7 +3196,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A10" s="10">
         <v>45510.306761192129</v>
       </c>
@@ -3318,7 +3341,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A11" s="10">
         <v>45517.312436354172</v>
       </c>
@@ -3463,7 +3486,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A12" s="10">
         <v>45527.50237717593</v>
       </c>
@@ -3608,7 +3631,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A13" s="10">
         <v>45527.505888935186</v>
       </c>
@@ -3753,7 +3776,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A14" s="10">
         <v>45517.552074386578</v>
       </c>
@@ -3898,7 +3921,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A15" s="10">
         <v>45517.554953865736</v>
       </c>
@@ -4043,7 +4066,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A16" s="10">
         <v>45517.556153761572</v>
       </c>

</xml_diff>

<commit_message>
Update Copy of IS Observation Form 2024 (Responses).xlsx
-finished the 1-16 times data
</commit_message>
<xml_diff>
--- a/Copy of IS Observation Form 2024 (Responses).xlsx
+++ b/Copy of IS Observation Form 2024 (Responses).xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nabtang\Documents\GitHub\IS-Observation-Form-2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IS-Observation-Form-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF647532-D9A7-48A9-81D0-D21FE98FE21C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Form Responses 1'!$E$1:$E$441</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,12 +33,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="AN21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="AN21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AR21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="AR21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -65,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="AS21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -78,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D81" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="D81" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -91,7 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E81" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="E81" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -109,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4346" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4355" uniqueCount="461">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1494,13 +1493,28 @@
   <si>
     <t>Phone Addicted Female ()</t>
   </si>
+  <si>
+    <t>Non-Addicted</t>
+  </si>
+  <si>
+    <t>Addicted</t>
+  </si>
+  <si>
+    <t>1-16 times male</t>
+  </si>
+  <si>
+    <t>1-16 times female</t>
+  </si>
+  <si>
+    <t>1-16 times total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
+    <numFmt numFmtId="187" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -1534,7 +1548,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1583,6 +1597,12 @@
         <bgColor rgb="FFCFE2F3"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1596,7 +1616,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1607,7 +1627,7 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="187" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1622,6 +1642,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1836,15 +1857,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AZ441"/>
+  <dimension ref="A1:BC441"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AU1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AY14" sqref="AY14"/>
+      <selection pane="bottomLeft" activeCell="BB11" sqref="BB11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1874,9 +1895,10 @@
     <col min="51" max="51" width="28" customWidth="1"/>
     <col min="52" max="52" width="26.42578125" customWidth="1"/>
     <col min="53" max="53" width="18.85546875" customWidth="1"/>
+    <col min="54" max="55" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2022,7 +2044,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A2" s="10">
         <v>45509.701037893523</v>
       </c>
@@ -2172,8 +2194,14 @@
       <c r="AZ2" t="s">
         <v>455</v>
       </c>
+      <c r="BB2" t="s">
+        <v>456</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>457</v>
+      </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
         <v>45509.70180761574</v>
       </c>
@@ -2325,8 +2353,16 @@
         <f>COUNTIF(AW143:AW341,"&gt;=33")</f>
         <v>86</v>
       </c>
+      <c r="BB3">
+        <f>340-149</f>
+        <v>191</v>
+      </c>
+      <c r="BC3">
+        <f>SUM(AY3,AZ3)</f>
+        <v>149</v>
+      </c>
     </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
         <v>45510.305194814813</v>
       </c>
@@ -2470,8 +2506,14 @@
         <f t="shared" ref="AW4:AW67" si="0">SUM(G4:Q4)</f>
         <v>31</v>
       </c>
+      <c r="BB4" s="25" t="s">
+        <v>458</v>
+      </c>
+      <c r="BC4" s="25" t="s">
+        <v>458</v>
+      </c>
     </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
         <v>45510.305908900467</v>
       </c>
@@ -2615,8 +2657,16 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
+      <c r="BB5">
+        <f>COUNTIFS(AW2:AW142,"&lt;31",AM2:AM142,AM4)</f>
+        <v>14</v>
+      </c>
+      <c r="BC5" s="25">
+        <f>COUNTIFS(AW2:AW142,"&gt;=31",AM2:AM142,AM4)</f>
+        <v>14</v>
+      </c>
     </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A6" s="10">
         <v>45510.450860081022</v>
       </c>
@@ -2760,8 +2810,14 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
+      <c r="BB6" s="25" t="s">
+        <v>459</v>
+      </c>
+      <c r="BC6" s="25" t="s">
+        <v>459</v>
+      </c>
     </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A7" s="10">
         <v>45533.454514236109</v>
       </c>
@@ -2905,8 +2961,16 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
+      <c r="BB7">
+        <f>COUNTIFS(AW142:AW341,"&lt;33",AM142:AM341,AM145)</f>
+        <v>21</v>
+      </c>
+      <c r="BC7" s="25">
+        <f>COUNTIFS(AW142:AW341,"&gt;=33",AM142:AM341,AM145)</f>
+        <v>5</v>
+      </c>
     </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
         <v>45534.598930266206</v>
       </c>
@@ -3050,8 +3114,14 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
+      <c r="BB8" s="25" t="s">
+        <v>460</v>
+      </c>
+      <c r="BC8" s="25" t="s">
+        <v>460</v>
+      </c>
     </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
         <v>45510.304203993059</v>
       </c>
@@ -3195,8 +3265,16 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
+      <c r="BB9">
+        <f>SUM(BB5,BB7)</f>
+        <v>35</v>
+      </c>
+      <c r="BC9" s="25">
+        <f>SUM(BC5,BC7)</f>
+        <v>19</v>
+      </c>
     </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A10" s="10">
         <v>45510.306761192129</v>
       </c>
@@ -3340,8 +3418,11 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
+      <c r="BB10" t="s">
+        <v>460</v>
+      </c>
     </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A11" s="10">
         <v>45517.312436354172</v>
       </c>
@@ -3485,8 +3566,12 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
+      <c r="BB11">
+        <f>COUNTIF(AM2:AM341,AM4)</f>
+        <v>54</v>
+      </c>
     </row>
-    <row r="12" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A12" s="10">
         <v>45527.50237717593</v>
       </c>
@@ -3631,7 +3716,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A13" s="10">
         <v>45527.505888935186</v>
       </c>
@@ -3776,7 +3861,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A14" s="10">
         <v>45517.552074386578</v>
       </c>
@@ -3921,7 +4006,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A15" s="10">
         <v>45517.554953865736</v>
       </c>
@@ -4066,7 +4151,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A16" s="10">
         <v>45517.556153761572</v>
       </c>
@@ -55354,8 +55439,8 @@
       <c r="AS441" s="24"/>
     </row>
   </sheetData>
-  <autoFilter ref="E1:E441" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AU441">
+  <autoFilter ref="E1:E441">
+    <sortState ref="A2:AU441">
       <sortCondition descending="1" ref="E1:E441"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Last Update for Data
-Finished all the data
</commit_message>
<xml_diff>
--- a/Copy of IS Observation Form 2024 (Responses).xlsx
+++ b/Copy of IS Observation Form 2024 (Responses).xlsx
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4539" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4561" uniqueCount="573">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1795,6 +1795,54 @@
   </si>
   <si>
     <t>Anxiety</t>
+  </si>
+  <si>
+    <t>Loving Fam male</t>
+  </si>
+  <si>
+    <t>loving fam male</t>
+  </si>
+  <si>
+    <t>loving fam female</t>
+  </si>
+  <si>
+    <t>loving fam total</t>
+  </si>
+  <si>
+    <t>loving fam total(full)</t>
+  </si>
+  <si>
+    <t>moderate fam male</t>
+  </si>
+  <si>
+    <t>moderate fam female</t>
+  </si>
+  <si>
+    <t>moderate fam total</t>
+  </si>
+  <si>
+    <t>moderate fam total(full)</t>
+  </si>
+  <si>
+    <t>unloving fam male</t>
+  </si>
+  <si>
+    <t>unloving male</t>
+  </si>
+  <si>
+    <t>unloving female</t>
+  </si>
+  <si>
+    <t>unloving fam female</t>
+  </si>
+  <si>
+    <t>unloving fam total</t>
+  </si>
+  <si>
+    <t>unloving total</t>
+  </si>
+  <si>
+    <t>un loving fam total(full)</t>
   </si>
 </sst>
 </file>
@@ -11219,9 +11267,9 @@
   </sheetPr>
   <dimension ref="A1:CT441"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ1" zoomScale="74" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AS164" sqref="AS164"/>
+    <sheetView tabSelected="1" topLeftCell="BA1" zoomScale="87" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BE229" sqref="BE229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -52003,6 +52051,15 @@
         <f t="shared" si="41"/>
         <v>8</v>
       </c>
+      <c r="BD205" t="s">
+        <v>5</v>
+      </c>
+      <c r="BE205" t="s">
+        <v>557</v>
+      </c>
+      <c r="BF205" t="s">
+        <v>558</v>
+      </c>
       <c r="BH205">
         <f t="shared" si="42"/>
         <v>24</v>
@@ -52196,6 +52253,14 @@
         <f t="shared" si="41"/>
         <v>1</v>
       </c>
+      <c r="BE206">
+        <f>COUNTIFS(AW2:AW142,"&lt;31",F2:F142,F2)</f>
+        <v>54</v>
+      </c>
+      <c r="BF206">
+        <f>COUNTIFS(AW2:AW142,"&gt;=31",F2:F142,F2)</f>
+        <v>40</v>
+      </c>
       <c r="BH206">
         <f t="shared" si="42"/>
         <v>18</v>
@@ -52389,6 +52454,12 @@
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
+      <c r="BE207" t="s">
+        <v>559</v>
+      </c>
+      <c r="BF207" t="s">
+        <v>559</v>
+      </c>
       <c r="BH207">
         <f t="shared" si="42"/>
         <v>0</v>
@@ -52582,6 +52653,14 @@
         <f t="shared" si="41"/>
         <v>7</v>
       </c>
+      <c r="BE208">
+        <f>COUNTIFS(AW143:AW341,"&lt;33",F143:F341,F2)</f>
+        <v>76</v>
+      </c>
+      <c r="BF208">
+        <f>COUNTIFS(AW143:AW341,"&gt;=33",F143:F341,F2)</f>
+        <v>52</v>
+      </c>
       <c r="BH208">
         <f t="shared" si="42"/>
         <v>14</v>
@@ -52775,6 +52854,12 @@
         <f t="shared" si="41"/>
         <v>10</v>
       </c>
+      <c r="BE209" t="s">
+        <v>560</v>
+      </c>
+      <c r="BF209" t="s">
+        <v>560</v>
+      </c>
       <c r="BH209">
         <f t="shared" si="42"/>
         <v>20</v>
@@ -52968,6 +53053,14 @@
         <f t="shared" si="41"/>
         <v>8</v>
       </c>
+      <c r="BE210">
+        <f>SUM(BE206,BE208)</f>
+        <v>130</v>
+      </c>
+      <c r="BF210">
+        <f>SUM(BF206,BF208)</f>
+        <v>92</v>
+      </c>
       <c r="BH210">
         <f t="shared" si="42"/>
         <v>32</v>
@@ -53161,6 +53254,9 @@
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
+      <c r="BE211" t="s">
+        <v>561</v>
+      </c>
       <c r="BH211">
         <f t="shared" si="42"/>
         <v>8</v>
@@ -53354,6 +53450,10 @@
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
+      <c r="BE212">
+        <f>COUNTIF(F2:F341,F2)</f>
+        <v>222</v>
+      </c>
       <c r="BH212">
         <f t="shared" si="42"/>
         <v>18</v>
@@ -53547,6 +53647,12 @@
         <f t="shared" si="41"/>
         <v>13</v>
       </c>
+      <c r="BE213" t="s">
+        <v>562</v>
+      </c>
+      <c r="BF213" t="s">
+        <v>562</v>
+      </c>
       <c r="BH213">
         <f t="shared" si="42"/>
         <v>28</v>
@@ -53740,6 +53846,14 @@
         <f t="shared" si="41"/>
         <v>16</v>
       </c>
+      <c r="BE214">
+        <f>COUNTIFS(AW2:AW142,"&lt;31",F2:F142,F3)</f>
+        <v>23</v>
+      </c>
+      <c r="BF214">
+        <f>COUNTIFS(AW2:AW142,"&gt;=31",F2:F142,F3)</f>
+        <v>20</v>
+      </c>
       <c r="BH214">
         <f t="shared" si="42"/>
         <v>30</v>
@@ -53933,6 +54047,12 @@
         <f t="shared" si="41"/>
         <v>8</v>
       </c>
+      <c r="BE215" t="s">
+        <v>563</v>
+      </c>
+      <c r="BF215" t="s">
+        <v>563</v>
+      </c>
       <c r="BH215">
         <f t="shared" si="42"/>
         <v>18</v>
@@ -54126,6 +54246,14 @@
         <f t="shared" si="41"/>
         <v>1</v>
       </c>
+      <c r="BE216">
+        <f>COUNTIFS(AW143:AW341,"&lt;33",F143:F341,F3)</f>
+        <v>37</v>
+      </c>
+      <c r="BF216">
+        <f>COUNTIFS(AW143:AW341,"&gt;=33",F143:F341,F3)</f>
+        <v>30</v>
+      </c>
       <c r="BH216">
         <f t="shared" si="42"/>
         <v>4</v>
@@ -54319,6 +54447,12 @@
         <f t="shared" si="41"/>
         <v>5</v>
       </c>
+      <c r="BE217" t="s">
+        <v>564</v>
+      </c>
+      <c r="BF217" t="s">
+        <v>564</v>
+      </c>
       <c r="BH217">
         <f t="shared" si="42"/>
         <v>20</v>
@@ -54512,6 +54646,14 @@
         <f t="shared" si="41"/>
         <v>3</v>
       </c>
+      <c r="BE218">
+        <f>SUM(BE214,BE216)</f>
+        <v>60</v>
+      </c>
+      <c r="BF218">
+        <f>SUM(BF214,BF216)</f>
+        <v>50</v>
+      </c>
       <c r="BH218">
         <f t="shared" si="42"/>
         <v>24</v>
@@ -54705,6 +54847,9 @@
         <f t="shared" si="41"/>
         <v>1</v>
       </c>
+      <c r="BE219" t="s">
+        <v>565</v>
+      </c>
       <c r="BH219">
         <f t="shared" si="42"/>
         <v>8</v>
@@ -54898,6 +55043,10 @@
         <f t="shared" si="41"/>
         <v>4</v>
       </c>
+      <c r="BE220">
+        <f>COUNTIF(F2:F341,F3)</f>
+        <v>110</v>
+      </c>
       <c r="BH220">
         <f t="shared" si="42"/>
         <v>10</v>
@@ -55091,6 +55240,12 @@
         <f t="shared" si="41"/>
         <v>1</v>
       </c>
+      <c r="BE221" t="s">
+        <v>566</v>
+      </c>
+      <c r="BF221" t="s">
+        <v>567</v>
+      </c>
       <c r="BH221">
         <f t="shared" si="42"/>
         <v>16</v>
@@ -55284,6 +55439,14 @@
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
+      <c r="BE222">
+        <f>COUNTIFS(AW2:AW142,"&lt;31",F2:F142,F19)</f>
+        <v>1</v>
+      </c>
+      <c r="BF222">
+        <f>COUNTIFS(AW2:AW142,"&gt;=31",F2:F142,F19)</f>
+        <v>3</v>
+      </c>
       <c r="BH222">
         <f t="shared" si="42"/>
         <v>10</v>
@@ -55477,6 +55640,12 @@
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
+      <c r="BE223" t="s">
+        <v>569</v>
+      </c>
+      <c r="BF223" t="s">
+        <v>568</v>
+      </c>
       <c r="BH223">
         <f t="shared" si="42"/>
         <v>12</v>
@@ -55670,6 +55839,14 @@
         <f t="shared" si="41"/>
         <v>9</v>
       </c>
+      <c r="BE224">
+        <f>COUNTIFS(AW143:AW341,"&lt;33",F143:F341,F19)</f>
+        <v>0</v>
+      </c>
+      <c r="BF224">
+        <f>COUNTIFS(AW143:AW341,"&gt;=33",F143:F341,F19)</f>
+        <v>4</v>
+      </c>
       <c r="BH224">
         <f t="shared" si="42"/>
         <v>16</v>
@@ -55863,6 +56040,12 @@
         <f t="shared" si="41"/>
         <v>14</v>
       </c>
+      <c r="BE225" t="s">
+        <v>570</v>
+      </c>
+      <c r="BF225" t="s">
+        <v>571</v>
+      </c>
       <c r="BH225">
         <f t="shared" si="42"/>
         <v>26</v>
@@ -56056,6 +56239,14 @@
         <f t="shared" si="41"/>
         <v>7</v>
       </c>
+      <c r="BE226">
+        <f>SUM(BE222,BE224)</f>
+        <v>1</v>
+      </c>
+      <c r="BF226">
+        <f>SUM(BF222,BF224)</f>
+        <v>7</v>
+      </c>
       <c r="BH226">
         <f t="shared" si="42"/>
         <v>14</v>
@@ -56249,6 +56440,9 @@
         <f t="shared" si="41"/>
         <v>2</v>
       </c>
+      <c r="BE227" t="s">
+        <v>572</v>
+      </c>
       <c r="BH227">
         <f t="shared" si="42"/>
         <v>16</v>
@@ -56441,6 +56635,10 @@
       <c r="AZ228">
         <f t="shared" si="41"/>
         <v>0</v>
+      </c>
+      <c r="BE228">
+        <f>COUNTIF(F2:F341,F19)</f>
+        <v>8</v>
       </c>
       <c r="BH228">
         <f t="shared" si="42"/>

</xml_diff>